<commit_message>
lots of minor tweaks and bugfixes: prices ending in .00 now display correctly and the script now notifies the user of how many of each type of tag paper is needed. Convenience script for Windows users now included
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -62,8 +62,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -130,8 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,15 +159,15 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="A2:L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A2:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
@@ -182,10 +187,10 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">

</xml_diff>

<commit_message>
minor rewrite: tag info now pulled from a database file instead of being manually entered by the user
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -20,18 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">SKU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal Price</t>
   </si>
   <si>
     <t xml:space="preserve">Sale Price</t>
@@ -157,40 +148,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A2:L41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -205,14 +195,34 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1001000</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor script adjustment, parts bin tags incoming
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -151,7 +151,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -198,7 +198,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1001000</v>
+        <v>1200586</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
extra commit just in case, branching off to test higher dpi/pdf output
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -148,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -210,7 +210,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>4</v>
@@ -219,10 +219,39 @@
         <v>5</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2302224</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skus can now be seperated by a '-', as per old radioshack tradition
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">Sale Price</t>
+    <t xml:space="preserve">price</t>
   </si>
   <si>
     <t xml:space="preserve">Small Tag Quantity</t>
@@ -47,15 +47,19 @@
   </si>
   <si>
     <t xml:space="preserve">Parts Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">273-1126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -122,12 +126,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,31 +158,32 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -197,26 +206,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1200586</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>0</v>
@@ -227,25 +236,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2302224</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
+        <v>2700217</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
changed the catalog and tag parser to include sale prices, users no longer need to manually enter sales
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
     <t xml:space="preserve">Small Tag Quantity</t>
   </si>
   <si>
@@ -47,19 +44,15 @@
   </si>
   <si>
     <t xml:space="preserve">Parts Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">273-1126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -126,16 +119,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -156,7 +145,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -165,25 +154,24 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -200,67 +188,6 @@
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2700217</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
syncing in all of the work I did on an untracked version of the writer, aslo adding a catalog prepper for when prices change
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -124,7 +124,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,7 +154,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>

</xml_diff>

<commit_message>
really quick fused tagwriter 1.01 and the latest tagwriter, currently uses number of arguments to determine whether to operate in standard or custom mode
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -145,10 +145,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -190,6 +190,32 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>2302218</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>